<commit_message>
more time series analysis
</commit_message>
<xml_diff>
--- a/data/09-21_total.xlsx
+++ b/data/09-21_total.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\data_science\Insurance_report\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E47EA7D-5AC0-4E0C-BD8C-CD26E563B369}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{323E7AE7-8F64-48F1-A95D-26D1C8AA2A02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3420" yWindow="3610" windowWidth="28800" windowHeight="15370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="09-21全国" sheetId="1" r:id="rId1"/>
@@ -641,7 +641,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19">
+  <numFmts count="1">
+    <numFmt numFmtId="168" formatCode="0.0"/>
+  </numFmts>
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -799,6 +802,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -1227,11 +1237,17 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1591,8 +1607,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R192"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="I87" sqref="I87"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3:R3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1600,6 +1616,17 @@
     <col min="1" max="1" width="52.90625" customWidth="1"/>
     <col min="2" max="2" width="28.81640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.90625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="22.26953125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.36328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="9" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.08984375" bestFit="1" customWidth="1"/>
+    <col min="10" max="12" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.90625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18">
@@ -1714,60 +1741,60 @@
         <v>338154395.5</v>
       </c>
     </row>
-    <row r="3" spans="1:18">
+    <row r="3" spans="1:18" ht="15.5">
       <c r="A3" s="1">
         <v>39845</v>
       </c>
       <c r="B3" t="s">
         <v>19</v>
       </c>
-      <c r="C3">
-        <v>32767025.600000001</v>
-      </c>
-      <c r="D3">
-        <v>7185819.9000000004</v>
-      </c>
-      <c r="E3">
-        <v>25581205.699999999</v>
-      </c>
-      <c r="F3">
-        <v>23589945.899999999</v>
-      </c>
-      <c r="G3">
-        <v>1403958.6</v>
-      </c>
-      <c r="H3">
-        <v>587301.1</v>
-      </c>
-      <c r="I3">
-        <v>8235800.2000000002</v>
-      </c>
-      <c r="J3">
-        <v>3514472.2</v>
-      </c>
-      <c r="K3">
-        <v>4721328.0999999996</v>
-      </c>
-      <c r="L3">
-        <v>4029203.3</v>
-      </c>
-      <c r="M3">
-        <v>540848.1</v>
-      </c>
-      <c r="N3">
-        <v>151276.70000000001</v>
-      </c>
-      <c r="O3">
-        <v>2617023.4</v>
-      </c>
-      <c r="P3">
-        <v>100047101.3</v>
-      </c>
-      <c r="Q3">
-        <v>221784969.59999999</v>
-      </c>
-      <c r="R3">
-        <v>354347298</v>
+      <c r="C3" s="3">
+        <v>21231670.59</v>
+      </c>
+      <c r="D3" s="2">
+        <v>4649354.71</v>
+      </c>
+      <c r="E3" s="2">
+        <v>16582315.880000001</v>
+      </c>
+      <c r="F3" s="2">
+        <v>15443030.83</v>
+      </c>
+      <c r="G3" s="2">
+        <v>815765.34</v>
+      </c>
+      <c r="H3" s="2">
+        <v>323519.71000000002</v>
+      </c>
+      <c r="I3" s="2">
+        <v>5285888.72</v>
+      </c>
+      <c r="J3" s="2">
+        <v>2271490.0699999998</v>
+      </c>
+      <c r="K3" s="2">
+        <v>3014398.65</v>
+      </c>
+      <c r="L3" s="2">
+        <v>2577771.21</v>
+      </c>
+      <c r="M3" s="2">
+        <v>338816.87</v>
+      </c>
+      <c r="N3" s="2">
+        <v>97810.58</v>
+      </c>
+      <c r="O3" s="2">
+        <v>1678057.01</v>
+      </c>
+      <c r="P3" s="2">
+        <v>88846207.769999996</v>
+      </c>
+      <c r="Q3" s="2">
+        <v>220627736.03999999</v>
+      </c>
+      <c r="R3" s="2">
+        <v>342091505.5</v>
       </c>
     </row>
     <row r="4" spans="1:18">
@@ -10399,5 +10426,6 @@
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>